<commit_message>
check excel to do list tomorrow
</commit_message>
<xml_diff>
--- a/homework1-2 (answers).xlsx
+++ b/homework1-2 (answers).xlsx
@@ -979,7 +979,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -1250,13 +1250,10 @@
     <xf numFmtId="0" fontId="23" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="2" pivotButton="0" quotePrefix="0" xfId="1"/>
@@ -1888,22 +1885,22 @@
       <c r="D3" t="n">
         <v>30</v>
       </c>
-      <c r="E3" s="142">
+      <c r="E3" s="114">
         <f>DATE(B3,C3,D3)</f>
         <v/>
       </c>
-      <c r="F3" s="142">
+      <c r="F3" s="115">
         <f>WEEKDAY(E3)</f>
         <v/>
       </c>
-      <c r="G3" s="142">
+      <c r="G3" s="114">
         <f>EOMONTH(E3,1)</f>
         <v/>
       </c>
       <c r="H3" t="n">
         <v>2</v>
       </c>
-      <c r="I3" s="142">
+      <c r="I3" s="114">
         <f>DATE(B3,C3+2,D3)</f>
         <v/>
       </c>
@@ -1923,22 +1920,22 @@
       <c r="D4" t="n">
         <v>3</v>
       </c>
-      <c r="E4" s="142">
+      <c r="E4" s="114">
         <f>DATE(B4,C4,D4)</f>
         <v/>
       </c>
-      <c r="F4" s="142">
+      <c r="F4" s="115">
         <f>WEEKDAY(E4)</f>
         <v/>
       </c>
-      <c r="G4" s="142">
+      <c r="G4" s="114">
         <f>EOMONTH(E4,1)</f>
         <v/>
       </c>
       <c r="H4" t="n">
         <v>-3</v>
       </c>
-      <c r="I4" s="142">
+      <c r="I4" s="114">
         <f>DATE(B4,C4-3,D4)</f>
         <v/>
       </c>
@@ -1949,7 +1946,7 @@
           <t>Days Beween two dates?</t>
         </is>
       </c>
-      <c r="E5" s="142">
+      <c r="E5" s="115">
         <f>E3-E4</f>
         <v/>
       </c>
@@ -1961,7 +1958,7 @@
           <t>MOnthes Beween two dates?</t>
         </is>
       </c>
-      <c r="E6" s="142">
+      <c r="E6" s="115">
         <f>DATEDIF(E4,E3,"m")</f>
         <v/>
       </c>
@@ -1973,7 +1970,7 @@
           <t>Current time?</t>
         </is>
       </c>
-      <c r="B8" s="142">
+      <c r="B8" s="138">
         <f>NOW()</f>
         <v/>
       </c>
@@ -1982,7 +1979,7 @@
           <t>Hours</t>
         </is>
       </c>
-      <c r="D8" s="142">
+      <c r="D8" s="139">
         <f>HOUR(B8)</f>
         <v/>
       </c>
@@ -1991,7 +1988,7 @@
           <t>Minutes</t>
         </is>
       </c>
-      <c r="G8" s="142">
+      <c r="G8" s="139">
         <f>MINUTE(B8)</f>
         <v/>
       </c>
@@ -2078,7 +2075,7 @@
       <c r="C2" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="D2" s="142">
+      <c r="D2" s="8">
         <f>IF(C2&gt;50,B2*$G$4,IF(C2&gt;0,B2*$G$5,"On target"))</f>
         <v/>
       </c>
@@ -2103,7 +2100,7 @@
       <c r="C3" s="6" t="n">
         <v>-22</v>
       </c>
-      <c r="D3" s="142">
+      <c r="D3" s="8">
         <f>IF(C3&gt;50,B3*$G$4,IF(C3&gt;0,B3*$G$5,"On target"))</f>
         <v/>
       </c>
@@ -2128,7 +2125,7 @@
       <c r="C4" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="142">
+      <c r="D4" s="8">
         <f>IF(C4&gt;50,B4*$G$4,IF(C4&gt;0,B4*$G$5,"On target"))</f>
         <v/>
       </c>
@@ -2153,7 +2150,7 @@
       <c r="C5" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="D5" s="142">
+      <c r="D5" s="8">
         <f>IF(C5&gt;50,B5*$G$4,IF(C5&gt;0,B5*$G$5,"On target"))</f>
         <v/>
       </c>
@@ -2178,7 +2175,7 @@
       <c r="C6" s="6" t="n">
         <v>88</v>
       </c>
-      <c r="D6" s="142">
+      <c r="D6" s="8">
         <f>IF(C6&gt;50,B6*$G$4,IF(C6&gt;0,B6*$G$5,"On target"))</f>
         <v/>
       </c>
@@ -2195,7 +2192,7 @@
       <c r="C7" s="6" t="n">
         <v>19</v>
       </c>
-      <c r="D7" s="142">
+      <c r="D7" s="8">
         <f>IF(C7&gt;50,B7*$G$4,IF(C7&gt;0,B7*$G$5,"On target"))</f>
         <v/>
       </c>
@@ -2212,7 +2209,7 @@
       <c r="C8" s="6" t="n">
         <v>-56</v>
       </c>
-      <c r="D8" s="142">
+      <c r="D8" s="8">
         <f>IF(C8&gt;50,B8*$G$4,IF(C8&gt;0,B8*$G$5,"On target"))</f>
         <v/>
       </c>
@@ -2229,7 +2226,7 @@
       <c r="C9" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="D9" s="142">
+      <c r="D9" s="8">
         <f>IF(C9&gt;50,B9*$G$4,IF(C9&gt;0,B9*$G$5,"On target"))</f>
         <v/>
       </c>
@@ -2309,11 +2306,11 @@
       <c r="C19" t="n">
         <v>6</v>
       </c>
-      <c r="D19" s="142">
+      <c r="D19" s="12">
         <f>IF(C19&gt;8,B19/2,IF(AND(C19&gt;5,C19&lt;8),B19/1.5,B19))</f>
         <v/>
       </c>
-      <c r="E19" s="142">
+      <c r="E19" s="12">
         <f>IF(D19&lt;AVERAGE(D19:D24),"decommissioned","ok")</f>
         <v/>
       </c>
@@ -2330,11 +2327,11 @@
       <c r="C20" t="n">
         <v>12</v>
       </c>
-      <c r="D20" s="142">
+      <c r="D20" s="12">
         <f>IF(C20&gt;8,B20/2,IF(AND(C20&gt;5,C20&lt;8),B20/1.5,B20))</f>
         <v/>
       </c>
-      <c r="E20" s="142">
+      <c r="E20" s="12">
         <f>IF(D20&lt;AVERAGE(D20:D25),"decommissioned","ok")</f>
         <v/>
       </c>
@@ -2351,11 +2348,11 @@
       <c r="C21" t="n">
         <v>5</v>
       </c>
-      <c r="D21" s="142">
+      <c r="D21" s="12">
         <f>IF(C21&gt;8,B21/2,IF(AND(C21&gt;5,C21&lt;8),B21/1.5,B21))</f>
         <v/>
       </c>
-      <c r="E21" s="142">
+      <c r="E21" s="12">
         <f>IF(D21&lt;AVERAGE(D21:D26),"decommissioned","ok")</f>
         <v/>
       </c>
@@ -2372,11 +2369,11 @@
       <c r="C22" t="n">
         <v>7</v>
       </c>
-      <c r="D22" s="142">
+      <c r="D22" s="12">
         <f>IF(C22&gt;8,B22/2,IF(AND(C22&gt;5,C22&lt;8),B22/1.5,B22))</f>
         <v/>
       </c>
-      <c r="E22" s="142">
+      <c r="E22" s="12">
         <f>IF(D22&lt;AVERAGE(D22:D27),"decommissioned","ok")</f>
         <v/>
       </c>
@@ -2394,11 +2391,11 @@
       <c r="C23" t="n">
         <v>10</v>
       </c>
-      <c r="D23" s="142">
+      <c r="D23" s="12">
         <f>IF(C23&gt;8,B23/2,IF(AND(C23&gt;5,C23&lt;8),B23/1.5,B23))</f>
         <v/>
       </c>
-      <c r="E23" s="142">
+      <c r="E23" s="12">
         <f>IF(D23&lt;AVERAGE(D23:D28),"decommissioned","ok")</f>
         <v/>
       </c>
@@ -2415,11 +2412,11 @@
       <c r="C24" t="n">
         <v>3</v>
       </c>
-      <c r="D24" s="142">
+      <c r="D24" s="12">
         <f>IF(C24&gt;8,B24/2,IF(AND(C24&gt;5,C24&lt;8),B24/1.5,B24))</f>
         <v/>
       </c>
-      <c r="E24" s="142">
+      <c r="E24" s="12">
         <f>IF(D24&lt;AVERAGE(D24:D29),"decommissioned","ok")</f>
         <v/>
       </c>
@@ -2514,7 +2511,7 @@
         </is>
       </c>
       <c r="G5" s="20" t="n"/>
-      <c r="H5" s="143" t="inlineStr">
+      <c r="H5" s="142" t="inlineStr">
         <is>
           <t>Rates</t>
         </is>
@@ -2537,7 +2534,7 @@
           <t>Standard</t>
         </is>
       </c>
-      <c r="F6" s="144">
+      <c r="F6" s="143">
         <f>VLOOKUP(E6,RatesTable,2,FALSE)*D6</f>
         <v/>
       </c>
@@ -2547,7 +2544,7 @@
           <t>Standard</t>
         </is>
       </c>
-      <c r="I6" s="145" t="n">
+      <c r="I6" s="144" t="n">
         <v>50</v>
       </c>
       <c r="J6" s="19" t="n"/>
@@ -2567,7 +2564,7 @@
           <t>Standard</t>
         </is>
       </c>
-      <c r="F7" s="144">
+      <c r="F7" s="143">
         <f>VLOOKUP(E7,RatesTable,2,FALSE)*D7</f>
         <v/>
       </c>
@@ -2577,7 +2574,7 @@
           <t>Overtime</t>
         </is>
       </c>
-      <c r="I7" s="145" t="n">
+      <c r="I7" s="144" t="n">
         <v>75</v>
       </c>
       <c r="J7" s="19" t="n"/>
@@ -2597,7 +2594,7 @@
           <t>Standard</t>
         </is>
       </c>
-      <c r="F8" s="144">
+      <c r="F8" s="143">
         <f>VLOOKUP(E8,RatesTable,2,FALSE)*D8</f>
         <v/>
       </c>
@@ -2607,7 +2604,7 @@
           <t>Weekend</t>
         </is>
       </c>
-      <c r="I8" s="145" t="n">
+      <c r="I8" s="144" t="n">
         <v>100</v>
       </c>
       <c r="J8" s="19" t="n"/>
@@ -2627,7 +2624,7 @@
           <t>Overtime</t>
         </is>
       </c>
-      <c r="F9" s="144">
+      <c r="F9" s="143">
         <f>VLOOKUP(E9,RatesTable,2,FALSE)*D9</f>
         <v/>
       </c>
@@ -2637,7 +2634,7 @@
           <t>Wkend OT</t>
         </is>
       </c>
-      <c r="I9" s="145" t="n">
+      <c r="I9" s="144" t="n">
         <v>150</v>
       </c>
       <c r="J9" s="19" t="n"/>
@@ -2657,7 +2654,7 @@
           <t>Weekend</t>
         </is>
       </c>
-      <c r="F10" s="144">
+      <c r="F10" s="143">
         <f>VLOOKUP(E10,RatesTable,2,FALSE)*D10</f>
         <v/>
       </c>
@@ -2681,7 +2678,7 @@
           <t>Wkend OT</t>
         </is>
       </c>
-      <c r="F11" s="144">
+      <c r="F11" s="143">
         <f>VLOOKUP(E11,RatesTable,2,FALSE)*D11</f>
         <v/>
       </c>
@@ -2705,7 +2702,7 @@
           <t>Wkend OT</t>
         </is>
       </c>
-      <c r="F12" s="144">
+      <c r="F12" s="143">
         <f>VLOOKUP(E12,RatesTable,2,FALSE)*D12</f>
         <v/>
       </c>
@@ -2729,7 +2726,7 @@
           <t>Standard</t>
         </is>
       </c>
-      <c r="F13" s="144">
+      <c r="F13" s="143">
         <f>VLOOKUP(E13,RatesTable,2,FALSE)*D13</f>
         <v/>
       </c>
@@ -2753,7 +2750,7 @@
           <t>Standard</t>
         </is>
       </c>
-      <c r="F14" s="144">
+      <c r="F14" s="143">
         <f>VLOOKUP(E14,RatesTable,2,FALSE)*D14</f>
         <v/>
       </c>
@@ -2777,7 +2774,7 @@
           <t>Standard</t>
         </is>
       </c>
-      <c r="F15" s="144">
+      <c r="F15" s="143">
         <f>VLOOKUP(E15,RatesTable,2,FALSE)*D15</f>
         <v/>
       </c>
@@ -2801,7 +2798,7 @@
           <t>Overtime</t>
         </is>
       </c>
-      <c r="F16" s="144">
+      <c r="F16" s="143">
         <f>VLOOKUP(E16,RatesTable,2,FALSE)*D16</f>
         <v/>
       </c>
@@ -2816,7 +2813,7 @@
       <c r="D17" s="20" t="n"/>
       <c r="E17" s="20" t="n"/>
       <c r="F17" s="20" t="n"/>
-      <c r="G17" s="146" t="n"/>
+      <c r="G17" s="145" t="n"/>
       <c r="H17" s="20" t="n"/>
       <c r="I17" s="20" t="n"/>
       <c r="J17" s="19" t="n"/>
@@ -2830,7 +2827,7 @@
           <t>Labour total</t>
         </is>
       </c>
-      <c r="F18" s="147">
+      <c r="F18" s="146">
         <f>SUM(F6:F16)</f>
         <v/>
       </c>
@@ -2856,13 +2853,13 @@
           <t>OVH (overheads)</t>
         </is>
       </c>
-      <c r="D23" s="148" t="n">
+      <c r="D23" s="147" t="n">
         <v>514</v>
       </c>
-      <c r="E23" s="149" t="n">
+      <c r="E23" s="148" t="n">
         <v>652</v>
       </c>
-      <c r="F23" s="150" t="n">
+      <c r="F23" s="149" t="n">
         <v>11</v>
       </c>
       <c r="G23" s="40" t="inlineStr">
@@ -2878,13 +2875,13 @@
           <t>MAT (material)</t>
         </is>
       </c>
-      <c r="D24" s="151" t="n">
+      <c r="D24" s="150" t="n">
         <v>18</v>
       </c>
-      <c r="E24" s="152" t="n">
+      <c r="E24" s="151" t="n">
         <v>569</v>
       </c>
-      <c r="F24" s="153" t="n">
+      <c r="F24" s="152" t="n">
         <v>174</v>
       </c>
       <c r="G24" s="40" t="inlineStr">
@@ -2900,13 +2897,13 @@
           <t>OGS (other goods/services)</t>
         </is>
       </c>
-      <c r="D25" s="154" t="n">
+      <c r="D25" s="153" t="n">
         <v>454</v>
       </c>
-      <c r="E25" s="152" t="n">
+      <c r="E25" s="151" t="n">
         <v>405</v>
       </c>
-      <c r="F25" s="153" t="n">
+      <c r="F25" s="152" t="n">
         <v>526</v>
       </c>
       <c r="G25" s="40" t="inlineStr">
@@ -2922,13 +2919,13 @@
           <t>SAL (salaries)</t>
         </is>
       </c>
-      <c r="D26" s="154" t="n">
+      <c r="D26" s="153" t="n">
         <v>451</v>
       </c>
-      <c r="E26" s="152" t="n">
+      <c r="E26" s="151" t="n">
         <v>657</v>
       </c>
-      <c r="F26" s="153" t="n">
+      <c r="F26" s="152" t="n">
         <v>905</v>
       </c>
       <c r="G26" s="40" t="inlineStr">
@@ -2944,13 +2941,13 @@
           <t>DEP (depreciation)</t>
         </is>
       </c>
-      <c r="D27" s="155" t="n">
+      <c r="D27" s="154" t="n">
         <v>261</v>
       </c>
-      <c r="E27" s="156" t="n">
+      <c r="E27" s="155" t="n">
         <v>34</v>
       </c>
-      <c r="F27" s="157" t="n">
+      <c r="F27" s="156" t="n">
         <v>708</v>
       </c>
       <c r="G27" s="40" t="inlineStr">
@@ -2966,13 +2963,13 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="D29" s="158" t="n">
+      <c r="D29" s="157" t="n">
         <v>1698</v>
       </c>
-      <c r="E29" s="158" t="n">
+      <c r="E29" s="157" t="n">
         <v>2317</v>
       </c>
-      <c r="F29" s="158" t="n">
+      <c r="F29" s="157" t="n">
         <v>2324</v>
       </c>
       <c r="G29" s="36" t="n"/>
@@ -3477,14 +3474,14 @@
       <c r="D2" s="83" t="n">
         <v>111</v>
       </c>
-      <c r="E2" s="159" t="n">
+      <c r="E2" s="158" t="n">
         <v>74</v>
       </c>
-      <c r="F2" s="160">
+      <c r="F2" s="159">
         <f>E2*0.2</f>
         <v/>
       </c>
-      <c r="G2" s="161">
+      <c r="G2" s="160">
         <f>D2*E2</f>
         <v/>
       </c>
@@ -3510,14 +3507,14 @@
       <c r="D3" s="91" t="n">
         <v>166</v>
       </c>
-      <c r="E3" s="162" t="n">
+      <c r="E3" s="161" t="n">
         <v>48</v>
       </c>
-      <c r="F3" s="162">
+      <c r="F3" s="161">
         <f>E3*0.2</f>
         <v/>
       </c>
-      <c r="G3" s="162">
+      <c r="G3" s="161">
         <f>D3*E3</f>
         <v/>
       </c>
@@ -3540,14 +3537,14 @@
       <c r="D4" s="91" t="n">
         <v>266</v>
       </c>
-      <c r="E4" s="162" t="n">
+      <c r="E4" s="161" t="n">
         <v>69</v>
       </c>
-      <c r="F4" s="162">
+      <c r="F4" s="161">
         <f>E4*0.2</f>
         <v/>
       </c>
-      <c r="G4" s="162">
+      <c r="G4" s="161">
         <f>D4*E4</f>
         <v/>
       </c>
@@ -3575,14 +3572,14 @@
       <c r="D5" s="91" t="n">
         <v>250</v>
       </c>
-      <c r="E5" s="162" t="n">
+      <c r="E5" s="161" t="n">
         <v>83</v>
       </c>
-      <c r="F5" s="162">
+      <c r="F5" s="161">
         <f>E5*0.2</f>
         <v/>
       </c>
-      <c r="G5" s="162">
+      <c r="G5" s="161">
         <f>D5*E5</f>
         <v/>
       </c>
@@ -3605,14 +3602,14 @@
       <c r="D6" s="91" t="n">
         <v>127</v>
       </c>
-      <c r="E6" s="162" t="n">
+      <c r="E6" s="161" t="n">
         <v>85</v>
       </c>
-      <c r="F6" s="162">
+      <c r="F6" s="161">
         <f>E6*0.2</f>
         <v/>
       </c>
-      <c r="G6" s="162">
+      <c r="G6" s="161">
         <f>D6*E6</f>
         <v/>
       </c>
@@ -3635,14 +3632,14 @@
       <c r="D7" s="91" t="n">
         <v>225</v>
       </c>
-      <c r="E7" s="162" t="n">
+      <c r="E7" s="161" t="n">
         <v>69</v>
       </c>
-      <c r="F7" s="162">
+      <c r="F7" s="161">
         <f>E7*0.2</f>
         <v/>
       </c>
-      <c r="G7" s="162">
+      <c r="G7" s="161">
         <f>D7*E7</f>
         <v/>
       </c>
@@ -3665,14 +3662,14 @@
       <c r="D8" s="91" t="n">
         <v>267</v>
       </c>
-      <c r="E8" s="162" t="n">
+      <c r="E8" s="161" t="n">
         <v>50</v>
       </c>
-      <c r="F8" s="162">
+      <c r="F8" s="161">
         <f>E8*0.2</f>
         <v/>
       </c>
-      <c r="G8" s="162">
+      <c r="G8" s="161">
         <f>D8*E8</f>
         <v/>
       </c>
@@ -3694,14 +3691,14 @@
       <c r="D9" s="91" t="n">
         <v>278</v>
       </c>
-      <c r="E9" s="162" t="n">
+      <c r="E9" s="161" t="n">
         <v>36</v>
       </c>
-      <c r="F9" s="162">
+      <c r="F9" s="161">
         <f>E9*0.2</f>
         <v/>
       </c>
-      <c r="G9" s="162">
+      <c r="G9" s="161">
         <f>D9*E9</f>
         <v/>
       </c>
@@ -3723,14 +3720,14 @@
       <c r="D10" s="91" t="n">
         <v>159</v>
       </c>
-      <c r="E10" s="162" t="n">
+      <c r="E10" s="161" t="n">
         <v>52</v>
       </c>
-      <c r="F10" s="162">
+      <c r="F10" s="161">
         <f>E10*0.2</f>
         <v/>
       </c>
-      <c r="G10" s="162">
+      <c r="G10" s="161">
         <f>D10*E10</f>
         <v/>
       </c>
@@ -3752,14 +3749,14 @@
       <c r="D11" s="91" t="n">
         <v>280</v>
       </c>
-      <c r="E11" s="162" t="n">
+      <c r="E11" s="161" t="n">
         <v>50</v>
       </c>
-      <c r="F11" s="162">
+      <c r="F11" s="161">
         <f>E11*0.2</f>
         <v/>
       </c>
-      <c r="G11" s="162">
+      <c r="G11" s="161">
         <f>D11*E11</f>
         <v/>
       </c>
@@ -3781,14 +3778,14 @@
       <c r="D12" s="91" t="n">
         <v>203</v>
       </c>
-      <c r="E12" s="162" t="n">
+      <c r="E12" s="161" t="n">
         <v>97</v>
       </c>
-      <c r="F12" s="162">
+      <c r="F12" s="161">
         <f>E12*0.2</f>
         <v/>
       </c>
-      <c r="G12" s="162">
+      <c r="G12" s="161">
         <f>D12*E12</f>
         <v/>
       </c>
@@ -3810,14 +3807,14 @@
       <c r="D13" s="91" t="n">
         <v>287</v>
       </c>
-      <c r="E13" s="162" t="n">
+      <c r="E13" s="161" t="n">
         <v>82</v>
       </c>
-      <c r="F13" s="162">
+      <c r="F13" s="161">
         <f>E13*0.2</f>
         <v/>
       </c>
-      <c r="G13" s="162">
+      <c r="G13" s="161">
         <f>D13*E13</f>
         <v/>
       </c>
@@ -3839,14 +3836,14 @@
       <c r="D14" s="91" t="n">
         <v>153</v>
       </c>
-      <c r="E14" s="162" t="n">
+      <c r="E14" s="161" t="n">
         <v>68</v>
       </c>
-      <c r="F14" s="162">
+      <c r="F14" s="161">
         <f>E14*0.2</f>
         <v/>
       </c>
-      <c r="G14" s="162">
+      <c r="G14" s="161">
         <f>D14*E14</f>
         <v/>
       </c>
@@ -3868,14 +3865,14 @@
       <c r="D15" s="91" t="n">
         <v>282</v>
       </c>
-      <c r="E15" s="162" t="n">
+      <c r="E15" s="161" t="n">
         <v>36</v>
       </c>
-      <c r="F15" s="162">
+      <c r="F15" s="161">
         <f>E15*0.2</f>
         <v/>
       </c>
-      <c r="G15" s="162">
+      <c r="G15" s="161">
         <f>D15*E15</f>
         <v/>
       </c>
@@ -3897,14 +3894,14 @@
       <c r="D16" s="91" t="n">
         <v>110</v>
       </c>
-      <c r="E16" s="162" t="n">
+      <c r="E16" s="161" t="n">
         <v>44</v>
       </c>
-      <c r="F16" s="162">
+      <c r="F16" s="161">
         <f>E16*0.2</f>
         <v/>
       </c>
-      <c r="G16" s="162">
+      <c r="G16" s="161">
         <f>D16*E16</f>
         <v/>
       </c>
@@ -3926,14 +3923,14 @@
       <c r="D17" s="91" t="n">
         <v>102</v>
       </c>
-      <c r="E17" s="162" t="n">
+      <c r="E17" s="161" t="n">
         <v>45</v>
       </c>
-      <c r="F17" s="162">
+      <c r="F17" s="161">
         <f>E17*0.2</f>
         <v/>
       </c>
-      <c r="G17" s="162">
+      <c r="G17" s="161">
         <f>D17*E17</f>
         <v/>
       </c>
@@ -3955,14 +3952,14 @@
       <c r="D18" s="91" t="n">
         <v>194</v>
       </c>
-      <c r="E18" s="162" t="n">
+      <c r="E18" s="161" t="n">
         <v>60</v>
       </c>
-      <c r="F18" s="162">
+      <c r="F18" s="161">
         <f>E18*0.2</f>
         <v/>
       </c>
-      <c r="G18" s="162">
+      <c r="G18" s="161">
         <f>D18*E18</f>
         <v/>
       </c>
@@ -3984,14 +3981,14 @@
       <c r="D19" s="91" t="n">
         <v>200</v>
       </c>
-      <c r="E19" s="162" t="n">
+      <c r="E19" s="161" t="n">
         <v>84</v>
       </c>
-      <c r="F19" s="162">
+      <c r="F19" s="161">
         <f>E19*0.2</f>
         <v/>
       </c>
-      <c r="G19" s="162">
+      <c r="G19" s="161">
         <f>D19*E19</f>
         <v/>
       </c>
@@ -4013,14 +4010,14 @@
       <c r="D20" s="91" t="n">
         <v>142</v>
       </c>
-      <c r="E20" s="162" t="n">
+      <c r="E20" s="161" t="n">
         <v>69</v>
       </c>
-      <c r="F20" s="162">
+      <c r="F20" s="161">
         <f>E20*0.2</f>
         <v/>
       </c>
-      <c r="G20" s="162">
+      <c r="G20" s="161">
         <f>D20*E20</f>
         <v/>
       </c>
@@ -4042,14 +4039,14 @@
       <c r="D21" s="91" t="n">
         <v>161</v>
       </c>
-      <c r="E21" s="162" t="n">
+      <c r="E21" s="161" t="n">
         <v>89</v>
       </c>
-      <c r="F21" s="162">
+      <c r="F21" s="161">
         <f>E21*0.2</f>
         <v/>
       </c>
-      <c r="G21" s="162">
+      <c r="G21" s="161">
         <f>D21*E21</f>
         <v/>
       </c>
@@ -4071,14 +4068,14 @@
       <c r="D22" s="91" t="n">
         <v>245</v>
       </c>
-      <c r="E22" s="162" t="n">
+      <c r="E22" s="161" t="n">
         <v>43</v>
       </c>
-      <c r="F22" s="162">
+      <c r="F22" s="161">
         <f>E22*0.2</f>
         <v/>
       </c>
-      <c r="G22" s="162">
+      <c r="G22" s="161">
         <f>D22*E22</f>
         <v/>
       </c>
@@ -4100,14 +4097,14 @@
       <c r="D23" s="91" t="n">
         <v>192</v>
       </c>
-      <c r="E23" s="162" t="n">
+      <c r="E23" s="161" t="n">
         <v>23</v>
       </c>
-      <c r="F23" s="162">
+      <c r="F23" s="161">
         <f>E23*0.2</f>
         <v/>
       </c>
-      <c r="G23" s="162">
+      <c r="G23" s="161">
         <f>D23*E23</f>
         <v/>
       </c>
@@ -4129,14 +4126,14 @@
       <c r="D24" s="91" t="n">
         <v>201</v>
       </c>
-      <c r="E24" s="162" t="n">
+      <c r="E24" s="161" t="n">
         <v>48</v>
       </c>
-      <c r="F24" s="162">
+      <c r="F24" s="161">
         <f>E24*0.2</f>
         <v/>
       </c>
-      <c r="G24" s="162">
+      <c r="G24" s="161">
         <f>D24*E24</f>
         <v/>
       </c>
@@ -4145,10 +4142,10 @@
       </c>
     </row>
     <row r="26">
-      <c r="F26" s="163" t="n"/>
+      <c r="F26" s="162" t="n"/>
     </row>
     <row r="27">
-      <c r="F27" s="163" t="n"/>
+      <c r="F27" s="162" t="n"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D24">
@@ -4299,14 +4296,14 @@
     </row>
     <row r="18" ht="15" customHeight="1" thickBot="1"/>
     <row r="19" ht="15" customHeight="1" thickBot="1">
-      <c r="B19" s="164" t="inlineStr">
+      <c r="B19" s="163" t="inlineStr">
         <is>
           <t>Resources Required per Pallet of Paneling Type</t>
         </is>
       </c>
-      <c r="C19" s="165" t="n"/>
-      <c r="D19" s="165" t="n"/>
-      <c r="E19" s="166" t="n"/>
+      <c r="C19" s="164" t="n"/>
+      <c r="D19" s="164" t="n"/>
+      <c r="E19" s="165" t="n"/>
       <c r="F19" s="104" t="n"/>
     </row>
     <row r="20">
@@ -4563,13 +4560,13 @@
       <c r="E2" s="109" t="n">
         <v>41974</v>
       </c>
-      <c r="F2" s="167" t="n">
+      <c r="F2" s="166" t="n">
         <v>3.75</v>
       </c>
       <c r="G2" s="64" t="n">
         <v>1500</v>
       </c>
-      <c r="H2" s="167">
+      <c r="H2" s="166">
         <f>Table24[[#This Row],[Price]]*Table24[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -4581,7 +4578,7 @@
       <c r="J2" t="n">
         <v>2456</v>
       </c>
-      <c r="K2" s="167" t="n">
+      <c r="K2" s="166" t="n">
         <v>300</v>
       </c>
     </row>
@@ -4603,13 +4600,13 @@
       <c r="E3" s="109" t="n">
         <v>41815</v>
       </c>
-      <c r="F3" s="167" t="n">
+      <c r="F3" s="166" t="n">
         <v>0.5</v>
       </c>
       <c r="G3" s="64" t="n">
         <v>4000</v>
       </c>
-      <c r="H3" s="167">
+      <c r="H3" s="166">
         <f>Table24[[#This Row],[Price]]*Table24[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -4621,7 +4618,7 @@
       <c r="J3" t="n">
         <v>21547</v>
       </c>
-      <c r="K3" s="167" t="n">
+      <c r="K3" s="166" t="n">
         <v>2000</v>
       </c>
     </row>
@@ -4643,13 +4640,13 @@
       <c r="E4" s="109" t="n">
         <v>42255</v>
       </c>
-      <c r="F4" s="167" t="n">
+      <c r="F4" s="166" t="n">
         <v>0.5</v>
       </c>
       <c r="G4" s="64" t="n">
         <v>4000</v>
       </c>
-      <c r="H4" s="167">
+      <c r="H4" s="166">
         <f>Table24[[#This Row],[Price]]*Table24[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -4661,7 +4658,7 @@
       <c r="J4" t="n">
         <v>546780</v>
       </c>
-      <c r="K4" s="167" t="n">
+      <c r="K4" s="166" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -4683,13 +4680,13 @@
       <c r="E5" s="109" t="n">
         <v>42196</v>
       </c>
-      <c r="F5" s="167" t="n">
+      <c r="F5" s="166" t="n">
         <v>1.25</v>
       </c>
       <c r="G5" s="64" t="n">
         <v>540</v>
       </c>
-      <c r="H5" s="167">
+      <c r="H5" s="166">
         <f>Table24[[#This Row],[Price]]*Table24[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -4701,7 +4698,7 @@
       <c r="J5" t="n">
         <v>532140</v>
       </c>
-      <c r="K5" s="167" t="n">
+      <c r="K5" s="166" t="n">
         <v>500</v>
       </c>
     </row>
@@ -4723,13 +4720,13 @@
       <c r="E6" s="109" t="n">
         <v>42178</v>
       </c>
-      <c r="F6" s="167" t="n">
+      <c r="F6" s="166" t="n">
         <v>1.25</v>
       </c>
       <c r="G6" s="64" t="n">
         <v>1450</v>
       </c>
-      <c r="H6" s="167">
+      <c r="H6" s="166">
         <f>Table24[[#This Row],[Price]]*Table24[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -4741,7 +4738,7 @@
       <c r="J6" t="n">
         <v>530124</v>
       </c>
-      <c r="K6" s="167" t="n">
+      <c r="K6" s="166" t="n">
         <v>1300</v>
       </c>
     </row>
@@ -4763,13 +4760,13 @@
       <c r="E7" s="109" t="n">
         <v>42356</v>
       </c>
-      <c r="F7" s="167" t="n">
+      <c r="F7" s="166" t="n">
         <v>2.5</v>
       </c>
       <c r="G7" s="64" t="n">
         <v>600</v>
       </c>
-      <c r="H7" s="167">
+      <c r="H7" s="166">
         <f>Table24[[#This Row],[Price]]*Table24[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -4781,7 +4778,7 @@
       <c r="J7" t="n">
         <v>621450</v>
       </c>
-      <c r="K7" s="167" t="n">
+      <c r="K7" s="166" t="n">
         <v>875</v>
       </c>
     </row>
@@ -4803,13 +4800,13 @@
       <c r="E8" s="109" t="n">
         <v>41916</v>
       </c>
-      <c r="F8" s="167" t="n">
+      <c r="F8" s="166" t="n">
         <v>0.75</v>
       </c>
       <c r="G8" s="64" t="n">
         <v>230</v>
       </c>
-      <c r="H8" s="167">
+      <c r="H8" s="166">
         <f>Table24[[#This Row],[Price]]*Table24[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -4821,7 +4818,7 @@
       <c r="J8" t="n">
         <v>22450</v>
       </c>
-      <c r="K8" s="167" t="n">
+      <c r="K8" s="166" t="n">
         <v>125</v>
       </c>
     </row>
@@ -4843,13 +4840,13 @@
       <c r="E9" s="109" t="n">
         <v>42325</v>
       </c>
-      <c r="F9" s="167" t="n">
+      <c r="F9" s="166" t="n">
         <v>0.875</v>
       </c>
       <c r="G9" s="64" t="n">
         <v>580</v>
       </c>
-      <c r="H9" s="167">
+      <c r="H9" s="166">
         <f>Table24[[#This Row],[Price]]*Table24[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -4861,7 +4858,7 @@
       <c r="J9" t="n">
         <v>234456</v>
       </c>
-      <c r="K9" s="167" t="n">
+      <c r="K9" s="166" t="n">
         <v>587.5</v>
       </c>
     </row>
@@ -4883,13 +4880,13 @@
       <c r="E10" s="109" t="n">
         <v>42346</v>
       </c>
-      <c r="F10" s="167" t="n">
+      <c r="F10" s="166" t="n">
         <v>0.625</v>
       </c>
       <c r="G10" s="64" t="n">
         <v>453</v>
       </c>
-      <c r="H10" s="167">
+      <c r="H10" s="166">
         <f>Table24[[#This Row],[Price]]*Table24[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -4901,7 +4898,7 @@
       <c r="J10" t="n">
         <v>322156</v>
       </c>
-      <c r="K10" s="167" t="n">
+      <c r="K10" s="166" t="n">
         <v>230</v>
       </c>
     </row>
@@ -4923,13 +4920,13 @@
       <c r="E11" s="109" t="n">
         <v>42314</v>
       </c>
-      <c r="F11" s="167" t="n">
+      <c r="F11" s="166" t="n">
         <v>0.25</v>
       </c>
       <c r="G11" s="64" t="n">
         <v>800</v>
       </c>
-      <c r="H11" s="167">
+      <c r="H11" s="166">
         <f>Table24[[#This Row],[Price]]*Table24[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -4941,7 +4938,7 @@
       <c r="J11" t="n">
         <v>34458</v>
       </c>
-      <c r="K11" s="167" t="n">
+      <c r="K11" s="166" t="n">
         <v>35</v>
       </c>
     </row>
@@ -4963,13 +4960,13 @@
       <c r="E12" s="109" t="n">
         <v>42302</v>
       </c>
-      <c r="F12" s="167" t="n">
+      <c r="F12" s="166" t="n">
         <v>5</v>
       </c>
       <c r="G12" s="64" t="n">
         <v>9000</v>
       </c>
-      <c r="H12" s="167">
+      <c r="H12" s="166">
         <f>Table24[[#This Row],[Price]]*Table24[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -4981,7 +4978,7 @@
       <c r="J12" t="n">
         <v>215889</v>
       </c>
-      <c r="K12" s="167" t="n">
+      <c r="K12" s="166" t="n">
         <v>37500</v>
       </c>
     </row>
@@ -5003,13 +5000,13 @@
       <c r="E13" s="109" t="n">
         <v>42236</v>
       </c>
-      <c r="F13" s="167" t="n">
+      <c r="F13" s="166" t="n">
         <v>5.25</v>
       </c>
       <c r="G13" s="64" t="n">
         <v>200</v>
       </c>
-      <c r="H13" s="167">
+      <c r="H13" s="166">
         <f>Table24[[#This Row],[Price]]*Table24[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -5021,7 +5018,7 @@
       <c r="J13" t="n">
         <v>244569</v>
       </c>
-      <c r="K13" s="167" t="n">
+      <c r="K13" s="166" t="n">
         <v>575</v>
       </c>
     </row>
@@ -5043,13 +5040,13 @@
       <c r="E14" s="109" t="n">
         <v>41905</v>
       </c>
-      <c r="F14" s="167" t="n">
+      <c r="F14" s="166" t="n">
         <v>5.375</v>
       </c>
       <c r="G14" s="64" t="n">
         <v>1400</v>
       </c>
-      <c r="H14" s="167">
+      <c r="H14" s="166">
         <f>Table24[[#This Row],[Price]]*Table24[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -5061,7 +5058,7 @@
       <c r="J14" t="n">
         <v>265447</v>
       </c>
-      <c r="K14" s="167" t="n">
+      <c r="K14" s="166" t="n">
         <v>3750</v>
       </c>
     </row>
@@ -5083,13 +5080,13 @@
       <c r="E15" s="109" t="n">
         <v>41856</v>
       </c>
-      <c r="F15" s="167" t="n">
+      <c r="F15" s="166" t="n">
         <v>5.5</v>
       </c>
       <c r="G15" s="64" t="n">
         <v>350</v>
       </c>
-      <c r="H15" s="167">
+      <c r="H15" s="166">
         <f>Table24[[#This Row],[Price]]*Table24[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -5101,7 +5098,7 @@
       <c r="J15" t="n">
         <v>45569</v>
       </c>
-      <c r="K15" s="167" t="n">
+      <c r="K15" s="166" t="n">
         <v>1300</v>
       </c>
     </row>
@@ -5123,13 +5120,13 @@
       <c r="E16" s="109" t="n">
         <v>41877</v>
       </c>
-      <c r="F16" s="167" t="n">
+      <c r="F16" s="166" t="n">
         <v>0.425</v>
       </c>
       <c r="G16" s="64" t="n">
         <v>600</v>
       </c>
-      <c r="H16" s="167">
+      <c r="H16" s="166">
         <f>Table24[[#This Row],[Price]]*Table24[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -5141,7 +5138,7 @@
       <c r="J16" t="n">
         <v>3325554</v>
       </c>
-      <c r="K16" s="167" t="n">
+      <c r="K16" s="166" t="n">
         <v>155</v>
       </c>
     </row>
@@ -5163,13 +5160,13 @@
       <c r="E17" s="109" t="n">
         <v>42296</v>
       </c>
-      <c r="F17" s="167" t="n">
+      <c r="F17" s="166" t="n">
         <v>2</v>
       </c>
       <c r="G17" s="64" t="n">
         <v>840</v>
       </c>
-      <c r="H17" s="167">
+      <c r="H17" s="166">
         <f>Table24[[#This Row],[Price]]*Table24[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -5181,7 +5178,7 @@
       <c r="J17" t="n">
         <v>24489</v>
       </c>
-      <c r="K17" s="167" t="n">
+      <c r="K17" s="166" t="n">
         <v>587.5</v>
       </c>
     </row>
@@ -5203,13 +5200,13 @@
       <c r="E18" s="109" t="n">
         <v>42131</v>
       </c>
-      <c r="F18" s="167" t="n">
+      <c r="F18" s="166" t="n">
         <v>7</v>
       </c>
       <c r="G18" s="64" t="n">
         <v>230</v>
       </c>
-      <c r="H18" s="167">
+      <c r="H18" s="166">
         <f>Table24[[#This Row],[Price]]*Table24[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -5221,7 +5218,7 @@
       <c r="J18" t="n">
         <v>255630</v>
       </c>
-      <c r="K18" s="167" t="n">
+      <c r="K18" s="166" t="n">
         <v>1500</v>
       </c>
     </row>
@@ -5243,13 +5240,13 @@
       <c r="E19" s="109" t="n">
         <v>42338</v>
       </c>
-      <c r="F19" s="167" t="n">
+      <c r="F19" s="166" t="n">
         <v>8.75</v>
       </c>
       <c r="G19" s="64" t="n">
         <v>210</v>
       </c>
-      <c r="H19" s="167">
+      <c r="H19" s="166">
         <f>Table24[[#This Row],[Price]]*Table24[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -5261,7 +5258,7 @@
       <c r="J19" t="n">
         <v>452130</v>
       </c>
-      <c r="K19" s="167" t="n">
+      <c r="K19" s="166" t="n">
         <v>1140</v>
       </c>
     </row>
@@ -5516,13 +5513,13 @@
       <c r="E2" s="109" t="n">
         <v>41974</v>
       </c>
-      <c r="F2" s="167" t="n">
+      <c r="F2" s="166" t="n">
         <v>3.75</v>
       </c>
       <c r="G2" s="64" t="n">
         <v>1500</v>
       </c>
-      <c r="H2" s="167">
+      <c r="H2" s="166">
         <f>Table243[[#This Row],[Price]]*Table243[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -5534,7 +5531,7 @@
       <c r="J2" t="n">
         <v>2456</v>
       </c>
-      <c r="K2" s="167" t="n">
+      <c r="K2" s="166" t="n">
         <v>300</v>
       </c>
     </row>
@@ -5556,13 +5553,13 @@
       <c r="E3" s="109" t="n">
         <v>41815</v>
       </c>
-      <c r="F3" s="167" t="n">
+      <c r="F3" s="166" t="n">
         <v>0.5</v>
       </c>
       <c r="G3" s="64" t="n">
         <v>4000</v>
       </c>
-      <c r="H3" s="167">
+      <c r="H3" s="166">
         <f>Table243[[#This Row],[Price]]*Table243[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -5574,7 +5571,7 @@
       <c r="J3" t="n">
         <v>21547</v>
       </c>
-      <c r="K3" s="167" t="n">
+      <c r="K3" s="166" t="n">
         <v>2000</v>
       </c>
     </row>
@@ -5596,13 +5593,13 @@
       <c r="E4" s="109" t="n">
         <v>42255</v>
       </c>
-      <c r="F4" s="167" t="n">
+      <c r="F4" s="166" t="n">
         <v>0.5</v>
       </c>
       <c r="G4" s="64" t="n">
         <v>4000</v>
       </c>
-      <c r="H4" s="167">
+      <c r="H4" s="166">
         <f>Table243[[#This Row],[Price]]*Table243[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -5614,7 +5611,7 @@
       <c r="J4" t="n">
         <v>546780</v>
       </c>
-      <c r="K4" s="167" t="n">
+      <c r="K4" s="166" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -5636,13 +5633,13 @@
       <c r="E5" s="109" t="n">
         <v>42196</v>
       </c>
-      <c r="F5" s="167" t="n">
+      <c r="F5" s="166" t="n">
         <v>1.25</v>
       </c>
       <c r="G5" s="64" t="n">
         <v>540</v>
       </c>
-      <c r="H5" s="167">
+      <c r="H5" s="166">
         <f>Table243[[#This Row],[Price]]*Table243[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -5654,7 +5651,7 @@
       <c r="J5" t="n">
         <v>532140</v>
       </c>
-      <c r="K5" s="167" t="n">
+      <c r="K5" s="166" t="n">
         <v>500</v>
       </c>
     </row>
@@ -5676,13 +5673,13 @@
       <c r="E6" s="109" t="n">
         <v>42178</v>
       </c>
-      <c r="F6" s="167" t="n">
+      <c r="F6" s="166" t="n">
         <v>1.25</v>
       </c>
       <c r="G6" s="64" t="n">
         <v>1450</v>
       </c>
-      <c r="H6" s="167">
+      <c r="H6" s="166">
         <f>Table243[[#This Row],[Price]]*Table243[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -5694,7 +5691,7 @@
       <c r="J6" t="n">
         <v>530124</v>
       </c>
-      <c r="K6" s="167" t="n">
+      <c r="K6" s="166" t="n">
         <v>1300</v>
       </c>
     </row>
@@ -5716,13 +5713,13 @@
       <c r="E7" s="109" t="n">
         <v>42356</v>
       </c>
-      <c r="F7" s="167" t="n">
+      <c r="F7" s="166" t="n">
         <v>2.5</v>
       </c>
       <c r="G7" s="64" t="n">
         <v>600</v>
       </c>
-      <c r="H7" s="167">
+      <c r="H7" s="166">
         <f>Table243[[#This Row],[Price]]*Table243[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -5734,7 +5731,7 @@
       <c r="J7" t="n">
         <v>621450</v>
       </c>
-      <c r="K7" s="167" t="n">
+      <c r="K7" s="166" t="n">
         <v>875</v>
       </c>
     </row>
@@ -5756,13 +5753,13 @@
       <c r="E8" s="109" t="n">
         <v>41916</v>
       </c>
-      <c r="F8" s="167" t="n">
+      <c r="F8" s="166" t="n">
         <v>0.75</v>
       </c>
       <c r="G8" s="64" t="n">
         <v>230</v>
       </c>
-      <c r="H8" s="167">
+      <c r="H8" s="166">
         <f>Table243[[#This Row],[Price]]*Table243[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -5774,7 +5771,7 @@
       <c r="J8" t="n">
         <v>22450</v>
       </c>
-      <c r="K8" s="167" t="n">
+      <c r="K8" s="166" t="n">
         <v>125</v>
       </c>
     </row>
@@ -5796,13 +5793,13 @@
       <c r="E9" s="109" t="n">
         <v>42325</v>
       </c>
-      <c r="F9" s="167" t="n">
+      <c r="F9" s="166" t="n">
         <v>0.875</v>
       </c>
       <c r="G9" s="64" t="n">
         <v>580</v>
       </c>
-      <c r="H9" s="167">
+      <c r="H9" s="166">
         <f>Table243[[#This Row],[Price]]*Table243[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -5814,7 +5811,7 @@
       <c r="J9" t="n">
         <v>234456</v>
       </c>
-      <c r="K9" s="167" t="n">
+      <c r="K9" s="166" t="n">
         <v>587.5</v>
       </c>
     </row>
@@ -5836,13 +5833,13 @@
       <c r="E10" s="109" t="n">
         <v>42346</v>
       </c>
-      <c r="F10" s="167" t="n">
+      <c r="F10" s="166" t="n">
         <v>0.625</v>
       </c>
       <c r="G10" s="64" t="n">
         <v>453</v>
       </c>
-      <c r="H10" s="167">
+      <c r="H10" s="166">
         <f>Table243[[#This Row],[Price]]*Table243[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -5854,7 +5851,7 @@
       <c r="J10" t="n">
         <v>322156</v>
       </c>
-      <c r="K10" s="167" t="n">
+      <c r="K10" s="166" t="n">
         <v>230</v>
       </c>
     </row>
@@ -5876,13 +5873,13 @@
       <c r="E11" s="109" t="n">
         <v>42314</v>
       </c>
-      <c r="F11" s="167" t="n">
+      <c r="F11" s="166" t="n">
         <v>0.25</v>
       </c>
       <c r="G11" s="64" t="n">
         <v>800</v>
       </c>
-      <c r="H11" s="167">
+      <c r="H11" s="166">
         <f>Table243[[#This Row],[Price]]*Table243[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -5894,7 +5891,7 @@
       <c r="J11" t="n">
         <v>34458</v>
       </c>
-      <c r="K11" s="167" t="n">
+      <c r="K11" s="166" t="n">
         <v>35</v>
       </c>
     </row>
@@ -5916,13 +5913,13 @@
       <c r="E12" s="109" t="n">
         <v>42302</v>
       </c>
-      <c r="F12" s="167" t="n">
+      <c r="F12" s="166" t="n">
         <v>5</v>
       </c>
       <c r="G12" s="64" t="n">
         <v>9000</v>
       </c>
-      <c r="H12" s="167">
+      <c r="H12" s="166">
         <f>Table243[[#This Row],[Price]]*Table243[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -5934,7 +5931,7 @@
       <c r="J12" t="n">
         <v>215889</v>
       </c>
-      <c r="K12" s="167" t="n">
+      <c r="K12" s="166" t="n">
         <v>37500</v>
       </c>
     </row>
@@ -5956,13 +5953,13 @@
       <c r="E13" s="109" t="n">
         <v>42236</v>
       </c>
-      <c r="F13" s="167" t="n">
+      <c r="F13" s="166" t="n">
         <v>5.25</v>
       </c>
       <c r="G13" s="64" t="n">
         <v>200</v>
       </c>
-      <c r="H13" s="167">
+      <c r="H13" s="166">
         <f>Table243[[#This Row],[Price]]*Table243[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -5974,7 +5971,7 @@
       <c r="J13" t="n">
         <v>244569</v>
       </c>
-      <c r="K13" s="167" t="n">
+      <c r="K13" s="166" t="n">
         <v>575</v>
       </c>
     </row>
@@ -5996,13 +5993,13 @@
       <c r="E14" s="109" t="n">
         <v>41905</v>
       </c>
-      <c r="F14" s="167" t="n">
+      <c r="F14" s="166" t="n">
         <v>5.375</v>
       </c>
       <c r="G14" s="64" t="n">
         <v>1400</v>
       </c>
-      <c r="H14" s="167">
+      <c r="H14" s="166">
         <f>Table243[[#This Row],[Price]]*Table243[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -6014,7 +6011,7 @@
       <c r="J14" t="n">
         <v>265447</v>
       </c>
-      <c r="K14" s="167" t="n">
+      <c r="K14" s="166" t="n">
         <v>3750</v>
       </c>
     </row>
@@ -6036,13 +6033,13 @@
       <c r="E15" s="109" t="n">
         <v>41856</v>
       </c>
-      <c r="F15" s="167" t="n">
+      <c r="F15" s="166" t="n">
         <v>5.5</v>
       </c>
       <c r="G15" s="64" t="n">
         <v>350</v>
       </c>
-      <c r="H15" s="167">
+      <c r="H15" s="166">
         <f>Table243[[#This Row],[Price]]*Table243[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -6054,7 +6051,7 @@
       <c r="J15" t="n">
         <v>45569</v>
       </c>
-      <c r="K15" s="167" t="n">
+      <c r="K15" s="166" t="n">
         <v>1300</v>
       </c>
     </row>
@@ -6076,13 +6073,13 @@
       <c r="E16" s="109" t="n">
         <v>41877</v>
       </c>
-      <c r="F16" s="167" t="n">
+      <c r="F16" s="166" t="n">
         <v>0.425</v>
       </c>
       <c r="G16" s="64" t="n">
         <v>600</v>
       </c>
-      <c r="H16" s="167">
+      <c r="H16" s="166">
         <f>Table243[[#This Row],[Price]]*Table243[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -6094,7 +6091,7 @@
       <c r="J16" t="n">
         <v>3325554</v>
       </c>
-      <c r="K16" s="167" t="n">
+      <c r="K16" s="166" t="n">
         <v>155</v>
       </c>
     </row>
@@ -6116,13 +6113,13 @@
       <c r="E17" s="109" t="n">
         <v>42296</v>
       </c>
-      <c r="F17" s="167" t="n">
+      <c r="F17" s="166" t="n">
         <v>2</v>
       </c>
       <c r="G17" s="64" t="n">
         <v>840</v>
       </c>
-      <c r="H17" s="167">
+      <c r="H17" s="166">
         <f>Table243[[#This Row],[Price]]*Table243[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -6134,7 +6131,7 @@
       <c r="J17" t="n">
         <v>24489</v>
       </c>
-      <c r="K17" s="167" t="n">
+      <c r="K17" s="166" t="n">
         <v>587.5</v>
       </c>
     </row>
@@ -6156,13 +6153,13 @@
       <c r="E18" s="109" t="n">
         <v>42131</v>
       </c>
-      <c r="F18" s="167" t="n">
+      <c r="F18" s="166" t="n">
         <v>7</v>
       </c>
       <c r="G18" s="64" t="n">
         <v>230</v>
       </c>
-      <c r="H18" s="167">
+      <c r="H18" s="166">
         <f>Table243[[#This Row],[Price]]*Table243[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -6174,7 +6171,7 @@
       <c r="J18" t="n">
         <v>255630</v>
       </c>
-      <c r="K18" s="167" t="n">
+      <c r="K18" s="166" t="n">
         <v>1500</v>
       </c>
     </row>
@@ -6196,13 +6193,13 @@
       <c r="E19" s="109" t="n">
         <v>42338</v>
       </c>
-      <c r="F19" s="167" t="n">
+      <c r="F19" s="166" t="n">
         <v>8.75</v>
       </c>
       <c r="G19" s="64" t="n">
         <v>210</v>
       </c>
-      <c r="H19" s="167">
+      <c r="H19" s="166">
         <f>Table243[[#This Row],[Price]]*Table243[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -6214,7 +6211,7 @@
       <c r="J19" t="n">
         <v>452130</v>
       </c>
-      <c r="K19" s="167" t="n">
+      <c r="K19" s="166" t="n">
         <v>1140</v>
       </c>
     </row>
@@ -6469,13 +6466,13 @@
       <c r="E2" s="109" t="n">
         <v>41974</v>
       </c>
-      <c r="F2" s="167" t="n">
+      <c r="F2" s="166" t="n">
         <v>3.75</v>
       </c>
       <c r="G2" s="64" t="n">
         <v>1500</v>
       </c>
-      <c r="H2" s="167">
+      <c r="H2" s="166">
         <f>Table2434[[#This Row],[Price]]*Table2434[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -6487,7 +6484,7 @@
       <c r="J2" t="n">
         <v>2456</v>
       </c>
-      <c r="K2" s="167" t="n">
+      <c r="K2" s="166" t="n">
         <v>300</v>
       </c>
     </row>
@@ -6509,13 +6506,13 @@
       <c r="E3" s="109" t="n">
         <v>41815</v>
       </c>
-      <c r="F3" s="167" t="n">
+      <c r="F3" s="166" t="n">
         <v>0.5</v>
       </c>
       <c r="G3" s="64" t="n">
         <v>4000</v>
       </c>
-      <c r="H3" s="167">
+      <c r="H3" s="166">
         <f>Table2434[[#This Row],[Price]]*Table2434[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -6527,7 +6524,7 @@
       <c r="J3" t="n">
         <v>21547</v>
       </c>
-      <c r="K3" s="167" t="n">
+      <c r="K3" s="166" t="n">
         <v>2000</v>
       </c>
     </row>
@@ -6549,13 +6546,13 @@
       <c r="E4" s="109" t="n">
         <v>42255</v>
       </c>
-      <c r="F4" s="167" t="n">
+      <c r="F4" s="166" t="n">
         <v>0.5</v>
       </c>
       <c r="G4" s="64" t="n">
         <v>4000</v>
       </c>
-      <c r="H4" s="167">
+      <c r="H4" s="166">
         <f>Table2434[[#This Row],[Price]]*Table2434[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -6567,7 +6564,7 @@
       <c r="J4" t="n">
         <v>546780</v>
       </c>
-      <c r="K4" s="167" t="n">
+      <c r="K4" s="166" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -6589,13 +6586,13 @@
       <c r="E5" s="109" t="n">
         <v>42196</v>
       </c>
-      <c r="F5" s="167" t="n">
+      <c r="F5" s="166" t="n">
         <v>1.25</v>
       </c>
       <c r="G5" s="64" t="n">
         <v>540</v>
       </c>
-      <c r="H5" s="167">
+      <c r="H5" s="166">
         <f>Table2434[[#This Row],[Price]]*Table2434[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -6607,7 +6604,7 @@
       <c r="J5" t="n">
         <v>532140</v>
       </c>
-      <c r="K5" s="167" t="n">
+      <c r="K5" s="166" t="n">
         <v>500</v>
       </c>
     </row>
@@ -6629,13 +6626,13 @@
       <c r="E6" s="109" t="n">
         <v>42178</v>
       </c>
-      <c r="F6" s="167" t="n">
+      <c r="F6" s="166" t="n">
         <v>1.25</v>
       </c>
       <c r="G6" s="64" t="n">
         <v>1450</v>
       </c>
-      <c r="H6" s="167">
+      <c r="H6" s="166">
         <f>Table2434[[#This Row],[Price]]*Table2434[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -6647,7 +6644,7 @@
       <c r="J6" t="n">
         <v>530124</v>
       </c>
-      <c r="K6" s="167" t="n">
+      <c r="K6" s="166" t="n">
         <v>1300</v>
       </c>
     </row>
@@ -6669,13 +6666,13 @@
       <c r="E7" s="109" t="n">
         <v>42356</v>
       </c>
-      <c r="F7" s="167" t="n">
+      <c r="F7" s="166" t="n">
         <v>2.5</v>
       </c>
       <c r="G7" s="64" t="n">
         <v>600</v>
       </c>
-      <c r="H7" s="167">
+      <c r="H7" s="166">
         <f>Table2434[[#This Row],[Price]]*Table2434[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -6687,7 +6684,7 @@
       <c r="J7" t="n">
         <v>621450</v>
       </c>
-      <c r="K7" s="167" t="n">
+      <c r="K7" s="166" t="n">
         <v>875</v>
       </c>
     </row>
@@ -6709,13 +6706,13 @@
       <c r="E8" s="109" t="n">
         <v>41916</v>
       </c>
-      <c r="F8" s="167" t="n">
+      <c r="F8" s="166" t="n">
         <v>0.75</v>
       </c>
       <c r="G8" s="64" t="n">
         <v>230</v>
       </c>
-      <c r="H8" s="167">
+      <c r="H8" s="166">
         <f>Table2434[[#This Row],[Price]]*Table2434[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -6727,7 +6724,7 @@
       <c r="J8" t="n">
         <v>22450</v>
       </c>
-      <c r="K8" s="167" t="n">
+      <c r="K8" s="166" t="n">
         <v>125</v>
       </c>
     </row>
@@ -6749,13 +6746,13 @@
       <c r="E9" s="109" t="n">
         <v>42325</v>
       </c>
-      <c r="F9" s="167" t="n">
+      <c r="F9" s="166" t="n">
         <v>0.875</v>
       </c>
       <c r="G9" s="64" t="n">
         <v>580</v>
       </c>
-      <c r="H9" s="167">
+      <c r="H9" s="166">
         <f>Table2434[[#This Row],[Price]]*Table2434[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -6767,7 +6764,7 @@
       <c r="J9" t="n">
         <v>234456</v>
       </c>
-      <c r="K9" s="167" t="n">
+      <c r="K9" s="166" t="n">
         <v>587.5</v>
       </c>
     </row>
@@ -6789,13 +6786,13 @@
       <c r="E10" s="109" t="n">
         <v>42346</v>
       </c>
-      <c r="F10" s="167" t="n">
+      <c r="F10" s="166" t="n">
         <v>0.625</v>
       </c>
       <c r="G10" s="64" t="n">
         <v>453</v>
       </c>
-      <c r="H10" s="167">
+      <c r="H10" s="166">
         <f>Table2434[[#This Row],[Price]]*Table2434[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -6807,7 +6804,7 @@
       <c r="J10" t="n">
         <v>322156</v>
       </c>
-      <c r="K10" s="167" t="n">
+      <c r="K10" s="166" t="n">
         <v>230</v>
       </c>
     </row>
@@ -6829,13 +6826,13 @@
       <c r="E11" s="109" t="n">
         <v>42314</v>
       </c>
-      <c r="F11" s="167" t="n">
+      <c r="F11" s="166" t="n">
         <v>0.25</v>
       </c>
       <c r="G11" s="64" t="n">
         <v>800</v>
       </c>
-      <c r="H11" s="167">
+      <c r="H11" s="166">
         <f>Table2434[[#This Row],[Price]]*Table2434[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -6847,7 +6844,7 @@
       <c r="J11" t="n">
         <v>34458</v>
       </c>
-      <c r="K11" s="167" t="n">
+      <c r="K11" s="166" t="n">
         <v>35</v>
       </c>
     </row>
@@ -6869,13 +6866,13 @@
       <c r="E12" s="109" t="n">
         <v>42302</v>
       </c>
-      <c r="F12" s="167" t="n">
+      <c r="F12" s="166" t="n">
         <v>5</v>
       </c>
       <c r="G12" s="64" t="n">
         <v>9000</v>
       </c>
-      <c r="H12" s="167">
+      <c r="H12" s="166">
         <f>Table2434[[#This Row],[Price]]*Table2434[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -6887,7 +6884,7 @@
       <c r="J12" t="n">
         <v>215889</v>
       </c>
-      <c r="K12" s="167" t="n">
+      <c r="K12" s="166" t="n">
         <v>37500</v>
       </c>
     </row>
@@ -6909,13 +6906,13 @@
       <c r="E13" s="109" t="n">
         <v>42236</v>
       </c>
-      <c r="F13" s="167" t="n">
+      <c r="F13" s="166" t="n">
         <v>5.25</v>
       </c>
       <c r="G13" s="64" t="n">
         <v>200</v>
       </c>
-      <c r="H13" s="167">
+      <c r="H13" s="166">
         <f>Table2434[[#This Row],[Price]]*Table2434[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -6927,7 +6924,7 @@
       <c r="J13" t="n">
         <v>244569</v>
       </c>
-      <c r="K13" s="167" t="n">
+      <c r="K13" s="166" t="n">
         <v>575</v>
       </c>
       <c r="M13">
@@ -6953,13 +6950,13 @@
       <c r="E14" s="109" t="n">
         <v>41905</v>
       </c>
-      <c r="F14" s="167" t="n">
+      <c r="F14" s="166" t="n">
         <v>5.375</v>
       </c>
       <c r="G14" s="64" t="n">
         <v>1400</v>
       </c>
-      <c r="H14" s="167">
+      <c r="H14" s="166">
         <f>Table2434[[#This Row],[Price]]*Table2434[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -6971,7 +6968,7 @@
       <c r="J14" t="n">
         <v>265447</v>
       </c>
-      <c r="K14" s="167" t="n">
+      <c r="K14" s="166" t="n">
         <v>3750</v>
       </c>
     </row>
@@ -6993,13 +6990,13 @@
       <c r="E15" s="109" t="n">
         <v>41856</v>
       </c>
-      <c r="F15" s="167" t="n">
+      <c r="F15" s="166" t="n">
         <v>5.5</v>
       </c>
       <c r="G15" s="64" t="n">
         <v>350</v>
       </c>
-      <c r="H15" s="167">
+      <c r="H15" s="166">
         <f>Table2434[[#This Row],[Price]]*Table2434[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -7011,7 +7008,7 @@
       <c r="J15" t="n">
         <v>45569</v>
       </c>
-      <c r="K15" s="167" t="n">
+      <c r="K15" s="166" t="n">
         <v>1300</v>
       </c>
     </row>
@@ -7033,13 +7030,13 @@
       <c r="E16" s="109" t="n">
         <v>41877</v>
       </c>
-      <c r="F16" s="167" t="n">
+      <c r="F16" s="166" t="n">
         <v>0.425</v>
       </c>
       <c r="G16" s="64" t="n">
         <v>600</v>
       </c>
-      <c r="H16" s="167">
+      <c r="H16" s="166">
         <f>Table2434[[#This Row],[Price]]*Table2434[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -7051,7 +7048,7 @@
       <c r="J16" t="n">
         <v>3325554</v>
       </c>
-      <c r="K16" s="167" t="n">
+      <c r="K16" s="166" t="n">
         <v>155</v>
       </c>
     </row>
@@ -7073,13 +7070,13 @@
       <c r="E17" s="109" t="n">
         <v>42296</v>
       </c>
-      <c r="F17" s="167" t="n">
+      <c r="F17" s="166" t="n">
         <v>2</v>
       </c>
       <c r="G17" s="64" t="n">
         <v>840</v>
       </c>
-      <c r="H17" s="167">
+      <c r="H17" s="166">
         <f>Table2434[[#This Row],[Price]]*Table2434[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -7091,7 +7088,7 @@
       <c r="J17" t="n">
         <v>24489</v>
       </c>
-      <c r="K17" s="167" t="n">
+      <c r="K17" s="166" t="n">
         <v>587.5</v>
       </c>
     </row>
@@ -7113,13 +7110,13 @@
       <c r="E18" s="109" t="n">
         <v>42131</v>
       </c>
-      <c r="F18" s="167" t="n">
+      <c r="F18" s="166" t="n">
         <v>7</v>
       </c>
       <c r="G18" s="64" t="n">
         <v>230</v>
       </c>
-      <c r="H18" s="167">
+      <c r="H18" s="166">
         <f>Table2434[[#This Row],[Price]]*Table2434[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -7131,7 +7128,7 @@
       <c r="J18" t="n">
         <v>255630</v>
       </c>
-      <c r="K18" s="167" t="n">
+      <c r="K18" s="166" t="n">
         <v>1500</v>
       </c>
     </row>
@@ -7153,13 +7150,13 @@
       <c r="E19" s="109" t="n">
         <v>42338</v>
       </c>
-      <c r="F19" s="167" t="n">
+      <c r="F19" s="166" t="n">
         <v>8.75</v>
       </c>
       <c r="G19" s="64" t="n">
         <v>210</v>
       </c>
-      <c r="H19" s="167">
+      <c r="H19" s="166">
         <f>Table2434[[#This Row],[Price]]*Table2434[[#This Row],[Quantity]]</f>
         <v/>
       </c>
@@ -7171,7 +7168,7 @@
       <c r="J19" t="n">
         <v>452130</v>
       </c>
-      <c r="K19" s="167" t="n">
+      <c r="K19" s="166" t="n">
         <v>1140</v>
       </c>
     </row>

</xml_diff>